<commit_message>
Rearange buttons in event popover.
</commit_message>
<xml_diff>
--- a/public/docs/nakladaci_list.xlsx
+++ b/public/docs/nakladaci_list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MiHu\Documents\projects\is-klost\is-klost\public\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MiHu\projects\is-klost\is-klost\public\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,15 +82,6 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -112,7 +103,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -139,19 +130,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normálne" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -167,7 +156,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motív Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -453,15 +442,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H70"/>
+  <dimension ref="A1:H193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="44.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
@@ -471,7 +458,7 @@
     <col min="8" max="8" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16"/>
       <c r="B1" s="16"/>
       <c r="C1" s="7"/>
@@ -492,8 +479,8 @@
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -502,8 +489,8 @@
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -522,8 +509,8 @@
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="5"/>
@@ -532,8 +519,8 @@
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="10"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
@@ -542,8 +529,8 @@
       <c r="H7" s="11"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
@@ -552,8 +539,8 @@
       <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
@@ -562,8 +549,8 @@
       <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -572,8 +559,8 @@
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -582,8 +569,8 @@
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -592,8 +579,8 @@
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -602,8 +589,8 @@
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -612,8 +599,8 @@
       <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -622,8 +609,8 @@
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -632,8 +619,8 @@
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -642,8 +629,8 @@
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -652,8 +639,8 @@
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -662,8 +649,8 @@
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -672,8 +659,8 @@
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -682,8 +669,8 @@
       <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -692,8 +679,8 @@
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -702,8 +689,8 @@
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -712,8 +699,8 @@
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -722,8 +709,8 @@
       <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -732,8 +719,8 @@
       <c r="H26" s="3"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -742,8 +729,8 @@
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="3"/>
@@ -752,8 +739,8 @@
       <c r="H28" s="14"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
@@ -762,8 +749,8 @@
       <c r="H29" s="15"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
@@ -772,8 +759,8 @@
       <c r="H30" s="6"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
+      <c r="A31" s="16"/>
+      <c r="B31" s="16"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
@@ -782,8 +769,8 @@
       <c r="H31" s="6"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
-      <c r="B32" s="17"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="16"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
@@ -792,8 +779,8 @@
       <c r="H32" s="6"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
-      <c r="B33" s="17"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="16"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -802,8 +789,8 @@
       <c r="H33" s="6"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="17"/>
-      <c r="B34" s="17"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="16"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
@@ -812,8 +799,8 @@
       <c r="H34" s="6"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
-      <c r="B35" s="21"/>
+      <c r="A35" s="18"/>
+      <c r="B35" s="18"/>
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -822,8 +809,8 @@
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
-      <c r="B36" s="22"/>
+      <c r="A36" s="18"/>
+      <c r="B36" s="18"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -832,8 +819,8 @@
       <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
-      <c r="B37" s="22"/>
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -842,8 +829,8 @@
       <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
-      <c r="B38" s="22"/>
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -852,8 +839,8 @@
       <c r="H38" s="2"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
-      <c r="B39" s="22"/>
+      <c r="A39" s="18"/>
+      <c r="B39" s="18"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -862,8 +849,8 @@
       <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
-      <c r="B40" s="22"/>
+      <c r="A40" s="18"/>
+      <c r="B40" s="18"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -872,8 +859,8 @@
       <c r="H40" s="2"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="21"/>
-      <c r="B41" s="21"/>
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -882,8 +869,8 @@
       <c r="H41" s="2"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
-      <c r="B42" s="22"/>
+      <c r="A42" s="18"/>
+      <c r="B42" s="18"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -892,8 +879,8 @@
       <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="18"/>
+      <c r="B43" s="18"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -902,8 +889,8 @@
       <c r="H43" s="2"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="18"/>
+      <c r="B44" s="18"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -912,8 +899,8 @@
       <c r="H44" s="2"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="18"/>
+      <c r="B45" s="18"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -922,8 +909,8 @@
       <c r="H45" s="2"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="22"/>
-      <c r="B46" s="22"/>
+      <c r="A46" s="18"/>
+      <c r="B46" s="18"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -932,8 +919,8 @@
       <c r="H46" s="2"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="22"/>
-      <c r="B47" s="22"/>
+      <c r="A47" s="18"/>
+      <c r="B47" s="18"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -942,8 +929,8 @@
       <c r="H47" s="2"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="22"/>
-      <c r="B48" s="22"/>
+      <c r="A48" s="18"/>
+      <c r="B48" s="18"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -952,8 +939,8 @@
       <c r="H48" s="2"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="22"/>
-      <c r="B49" s="22"/>
+      <c r="A49" s="18"/>
+      <c r="B49" s="18"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -962,8 +949,8 @@
       <c r="H49" s="2"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="22"/>
-      <c r="B50" s="22"/>
+      <c r="A50" s="18"/>
+      <c r="B50" s="18"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -972,8 +959,8 @@
       <c r="H50" s="2"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="22"/>
-      <c r="B51" s="22"/>
+      <c r="A51" s="18"/>
+      <c r="B51" s="18"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -982,8 +969,8 @@
       <c r="H51" s="2"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="22"/>
-      <c r="B52" s="22"/>
+      <c r="A52" s="18"/>
+      <c r="B52" s="18"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
@@ -992,8 +979,8 @@
       <c r="H52" s="3"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="22"/>
-      <c r="B53" s="22"/>
+      <c r="A53" s="18"/>
+      <c r="B53" s="18"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
@@ -1002,72 +989,564 @@
       <c r="H53" s="3"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="23"/>
-      <c r="B54" s="23"/>
+      <c r="A54" s="19"/>
+      <c r="B54" s="19"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="23"/>
-      <c r="B55" s="23"/>
+      <c r="A55" s="19"/>
+      <c r="B55" s="19"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="23"/>
-      <c r="B56" s="23"/>
+      <c r="A56" s="19"/>
+      <c r="B56" s="19"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="23"/>
-      <c r="B57" s="23"/>
+      <c r="A57" s="19"/>
+      <c r="B57" s="19"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="23"/>
-      <c r="B58" s="23"/>
+      <c r="A58" s="19"/>
+      <c r="B58" s="19"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="23"/>
-      <c r="B59" s="23"/>
+      <c r="A59" s="19"/>
+      <c r="B59" s="19"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="23"/>
-      <c r="B60" s="23"/>
+      <c r="A60" s="19"/>
+      <c r="B60" s="19"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="23"/>
-      <c r="B61" s="23"/>
+      <c r="A61" s="19"/>
+      <c r="B61" s="19"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="23"/>
-      <c r="B62" s="23"/>
+      <c r="A62" s="19"/>
+      <c r="B62" s="19"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="23"/>
-      <c r="B63" s="23"/>
+      <c r="A63" s="19"/>
+      <c r="B63" s="19"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="23"/>
-      <c r="B64" s="23"/>
+      <c r="A64" s="19"/>
+      <c r="B64" s="19"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="23"/>
-      <c r="B65" s="23"/>
+      <c r="A65" s="19"/>
+      <c r="B65" s="19"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="23"/>
-      <c r="B66" s="23"/>
+      <c r="A66" s="19"/>
+      <c r="B66" s="19"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="23"/>
-      <c r="B67" s="23"/>
+      <c r="A67" s="19"/>
+      <c r="B67" s="19"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="23"/>
-      <c r="B68" s="23"/>
+      <c r="A68" s="19"/>
+      <c r="B68" s="19"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="23"/>
-      <c r="B69" s="23"/>
+      <c r="A69" s="19"/>
+      <c r="B69" s="19"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="23"/>
-      <c r="B70" s="23"/>
+      <c r="A70" s="19"/>
+      <c r="B70" s="19"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="19"/>
+      <c r="B71" s="19"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="19"/>
+      <c r="B72" s="19"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="19"/>
+      <c r="B73" s="19"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="19"/>
+      <c r="B74" s="19"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="19"/>
+      <c r="B75" s="19"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="19"/>
+      <c r="B76" s="19"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="19"/>
+      <c r="B77" s="19"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="19"/>
+      <c r="B78" s="19"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="19"/>
+      <c r="B79" s="19"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="19"/>
+      <c r="B80" s="19"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="19"/>
+      <c r="B81" s="19"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="19"/>
+      <c r="B82" s="19"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="19"/>
+      <c r="B83" s="19"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="19"/>
+      <c r="B84" s="19"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="19"/>
+      <c r="B85" s="19"/>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="19"/>
+      <c r="B86" s="19"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="19"/>
+      <c r="B87" s="19"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="19"/>
+      <c r="B88" s="19"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="19"/>
+      <c r="B89" s="19"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="19"/>
+      <c r="B90" s="19"/>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="19"/>
+      <c r="B91" s="19"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="19"/>
+      <c r="B92" s="19"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="19"/>
+      <c r="B93" s="19"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="19"/>
+      <c r="B94" s="19"/>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="19"/>
+      <c r="B95" s="19"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="19"/>
+      <c r="B96" s="19"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="19"/>
+      <c r="B97" s="19"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="19"/>
+      <c r="B98" s="19"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="19"/>
+      <c r="B99" s="19"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="19"/>
+      <c r="B100" s="19"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="19"/>
+      <c r="B101" s="19"/>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="19"/>
+      <c r="B102" s="19"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="19"/>
+      <c r="B103" s="19"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="19"/>
+      <c r="B104" s="19"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="19"/>
+      <c r="B105" s="19"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="19"/>
+      <c r="B106" s="19"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="19"/>
+      <c r="B107" s="19"/>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="19"/>
+      <c r="B108" s="19"/>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="19"/>
+      <c r="B109" s="19"/>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="19"/>
+      <c r="B110" s="19"/>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="19"/>
+      <c r="B111" s="19"/>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="19"/>
+      <c r="B112" s="19"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="19"/>
+      <c r="B113" s="19"/>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="19"/>
+      <c r="B114" s="19"/>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="19"/>
+      <c r="B115" s="19"/>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="19"/>
+      <c r="B116" s="19"/>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="19"/>
+      <c r="B117" s="19"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="19"/>
+      <c r="B118" s="19"/>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="19"/>
+      <c r="B119" s="19"/>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="19"/>
+      <c r="B120" s="19"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="19"/>
+      <c r="B121" s="19"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="19"/>
+      <c r="B122" s="19"/>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="19"/>
+      <c r="B123" s="19"/>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="19"/>
+      <c r="B124" s="19"/>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="19"/>
+      <c r="B125" s="19"/>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="19"/>
+      <c r="B126" s="19"/>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="19"/>
+      <c r="B127" s="19"/>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="19"/>
+      <c r="B128" s="19"/>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="19"/>
+      <c r="B129" s="19"/>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="19"/>
+      <c r="B130" s="19"/>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="19"/>
+      <c r="B131" s="19"/>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="19"/>
+      <c r="B132" s="19"/>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="19"/>
+      <c r="B133" s="19"/>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="19"/>
+      <c r="B134" s="19"/>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="19"/>
+      <c r="B135" s="19"/>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="19"/>
+      <c r="B136" s="19"/>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="19"/>
+      <c r="B137" s="19"/>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="19"/>
+      <c r="B138" s="19"/>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="19"/>
+      <c r="B139" s="19"/>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="19"/>
+      <c r="B140" s="19"/>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="19"/>
+      <c r="B141" s="19"/>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="19"/>
+      <c r="B142" s="19"/>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="19"/>
+      <c r="B143" s="19"/>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="19"/>
+      <c r="B144" s="19"/>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="19"/>
+      <c r="B145" s="19"/>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="19"/>
+      <c r="B146" s="19"/>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="19"/>
+      <c r="B147" s="19"/>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="19"/>
+      <c r="B148" s="19"/>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="19"/>
+      <c r="B149" s="19"/>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="19"/>
+      <c r="B150" s="19"/>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="19"/>
+      <c r="B151" s="19"/>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="19"/>
+      <c r="B152" s="19"/>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="19"/>
+      <c r="B153" s="19"/>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="19"/>
+      <c r="B154" s="19"/>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="19"/>
+      <c r="B155" s="19"/>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="19"/>
+      <c r="B156" s="19"/>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="19"/>
+      <c r="B157" s="19"/>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="19"/>
+      <c r="B158" s="19"/>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="19"/>
+      <c r="B159" s="19"/>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="19"/>
+      <c r="B160" s="19"/>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="19"/>
+      <c r="B161" s="19"/>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" s="19"/>
+      <c r="B162" s="19"/>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="19"/>
+      <c r="B163" s="19"/>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="19"/>
+      <c r="B164" s="19"/>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" s="19"/>
+      <c r="B165" s="19"/>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="19"/>
+      <c r="B166" s="19"/>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="19"/>
+      <c r="B167" s="19"/>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" s="19"/>
+      <c r="B168" s="19"/>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" s="19"/>
+      <c r="B169" s="19"/>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" s="19"/>
+      <c r="B170" s="19"/>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" s="19"/>
+      <c r="B171" s="19"/>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="19"/>
+      <c r="B172" s="19"/>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="19"/>
+      <c r="B173" s="19"/>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" s="19"/>
+      <c r="B174" s="19"/>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" s="19"/>
+      <c r="B175" s="19"/>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" s="19"/>
+      <c r="B176" s="19"/>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" s="19"/>
+      <c r="B177" s="19"/>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" s="19"/>
+      <c r="B178" s="19"/>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" s="19"/>
+      <c r="B179" s="19"/>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" s="19"/>
+      <c r="B180" s="19"/>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" s="19"/>
+      <c r="B181" s="19"/>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" s="19"/>
+      <c r="B182" s="19"/>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" s="19"/>
+      <c r="B183" s="19"/>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" s="19"/>
+      <c r="B184" s="19"/>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" s="19"/>
+      <c r="B185" s="19"/>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" s="19"/>
+      <c r="B186" s="19"/>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" s="19"/>
+      <c r="B187" s="19"/>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" s="19"/>
+      <c r="B188" s="19"/>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" s="19"/>
+      <c r="B189" s="19"/>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" s="19"/>
+      <c r="B190" s="19"/>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" s="19"/>
+      <c r="B191" s="19"/>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" s="19"/>
+      <c r="B192" s="19"/>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" s="19"/>
+      <c r="B193" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.39370078740157483" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>